<commit_message>
Clean up directories - move 2018.2_AR71791 to 2018.2, add lime/shared, fix gaussian_delay.py.
</commit_message>
<xml_diff>
--- a/system/clocks_sidewinder.xlsx
+++ b/system/clocks_sidewinder.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="L:\work\lime\system\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\macaraeg1\Projects\comp\repositories\lime_axi_delayv\system\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6DAAA87-859A-4515-8DAB-A8E2C71F384C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C656D14-A699-4451-8BE0-2CC645A1D1E9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1545" yWindow="5085" windowWidth="18705" windowHeight="15555" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13620" yWindow="0" windowWidth="18780" windowHeight="20750" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -858,26 +858,28 @@
   </sheetPr>
   <dimension ref="A1:K108"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.7109375" customWidth="1"/>
-    <col min="2" max="2" width="10.85546875" customWidth="1"/>
-    <col min="3" max="3" width="10.5703125" customWidth="1"/>
-    <col min="4" max="4" width="10.42578125" customWidth="1"/>
+    <col min="1" max="1" width="19.7265625" customWidth="1"/>
+    <col min="2" max="2" width="10.81640625" customWidth="1"/>
+    <col min="3" max="3" width="10.54296875" customWidth="1"/>
+    <col min="4" max="4" width="10.453125" customWidth="1"/>
     <col min="5" max="5" width="11" customWidth="1"/>
-    <col min="6" max="6" width="10.140625" customWidth="1"/>
-    <col min="7" max="7" width="10.85546875" customWidth="1"/>
-    <col min="8" max="8" width="10.28515625" customWidth="1"/>
+    <col min="6" max="6" width="10.1796875" customWidth="1"/>
+    <col min="7" max="7" width="10.81640625" customWidth="1"/>
+    <col min="8" max="8" width="10.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" s="6" t="s">
         <v>0</v>
       </c>
@@ -889,13 +891,13 @@
         <v>63</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="F4" s="6"/>
       <c r="G4" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
         <v>3</v>
       </c>
@@ -917,7 +919,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>1</v>
       </c>
@@ -941,7 +943,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -965,7 +967,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>2</v>
       </c>
@@ -991,7 +993,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>86</v>
       </c>
@@ -1024,7 +1026,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>87</v>
       </c>
@@ -1057,7 +1059,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>88</v>
       </c>
@@ -1090,7 +1092,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>89</v>
       </c>
@@ -1123,7 +1125,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>90</v>
       </c>
@@ -1156,7 +1158,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>28</v>
       </c>
@@ -1186,12 +1188,12 @@
         <v>3.7499999999999999E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>3</v>
       </c>
@@ -1217,7 +1219,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>92</v>
       </c>
@@ -1247,7 +1249,7 @@
         <v>4.5454545454545456E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>103</v>
       </c>
@@ -1277,7 +1279,7 @@
         <v>0.36363636363636365</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>93</v>
       </c>
@@ -1310,7 +1312,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>94</v>
       </c>
@@ -1324,7 +1326,7 @@
         <v>7</v>
       </c>
       <c r="E23" s="7">
-        <f t="shared" ref="E22:E27" si="7">VLOOKUP($B23,$A$11:$F$16,5,FALSE)/$C23</f>
+        <f t="shared" ref="E23:E27" si="7">VLOOKUP($B23,$A$11:$F$16,5,FALSE)/$C23</f>
         <v>461.11111111111114</v>
       </c>
       <c r="F23" s="4">
@@ -1332,15 +1334,15 @@
         <v>2.1686746987951806</v>
       </c>
       <c r="G23" s="9">
-        <f t="shared" ref="G22:G35" si="8">$E23*$B$3</f>
+        <f t="shared" ref="G23:G35" si="8">$E23*$B$3</f>
         <v>9222.2222222222226</v>
       </c>
       <c r="H23" s="9">
-        <f t="shared" ref="H22:H35" si="9">$F23/$B$3</f>
+        <f t="shared" ref="H23:H35" si="9">$F23/$B$3</f>
         <v>0.10843373493975902</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>95</v>
       </c>
@@ -1370,7 +1372,7 @@
         <v>9.0909090909090912E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>96</v>
       </c>
@@ -1400,7 +1402,7 @@
         <v>9.0909090909090912E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>109</v>
       </c>
@@ -1430,7 +1432,7 @@
         <v>0.10843373493975902</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>110</v>
       </c>
@@ -1460,7 +1462,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>97</v>
       </c>
@@ -1468,29 +1470,29 @@
         <v>89</v>
       </c>
       <c r="C28" s="3">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D28" s="3">
         <v>1</v>
       </c>
       <c r="E28" s="7">
         <f>VLOOKUP($B28,$A$11:$F$16,5,FALSE)/$C28/$D28</f>
-        <v>250</v>
+        <v>187.5</v>
       </c>
       <c r="F28" s="4">
         <f t="shared" si="4"/>
-        <v>4</v>
+        <v>5.333333333333333</v>
       </c>
       <c r="G28" s="9">
         <f t="shared" si="8"/>
-        <v>5000</v>
+        <v>3750</v>
       </c>
       <c r="H28" s="9">
         <f t="shared" si="9"/>
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+        <v>0.26666666666666666</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>104</v>
       </c>
@@ -1520,7 +1522,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>98</v>
       </c>
@@ -1528,29 +1530,29 @@
         <v>89</v>
       </c>
       <c r="C30" s="3">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D30" s="3">
         <v>1</v>
       </c>
       <c r="E30" s="7">
         <f t="shared" ref="E30:E32" si="10">VLOOKUP($B30,$A$11:$F$16,5,FALSE)/$C30/$D30</f>
-        <v>300</v>
+        <v>187.5</v>
       </c>
       <c r="F30" s="4">
         <f t="shared" si="4"/>
-        <v>3.3333333333333335</v>
+        <v>5.333333333333333</v>
       </c>
       <c r="G30" s="9">
         <f t="shared" si="8"/>
-        <v>6000</v>
+        <v>3750</v>
       </c>
       <c r="H30" s="9">
         <f t="shared" si="9"/>
-        <v>0.16666666666666669</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+        <v>0.26666666666666666</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>99</v>
       </c>
@@ -1583,7 +1585,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>100</v>
       </c>
@@ -1616,7 +1618,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>107</v>
       </c>
@@ -1647,7 +1649,7 @@
         <v>5.4216867469879512E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>29</v>
       </c>
@@ -1678,7 +1680,7 @@
         <v>4.6875000000000014E-2</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>26</v>
       </c>
@@ -1709,7 +1711,7 @@
         <v>0.18750000000000006</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
         <v>10</v>
       </c>
@@ -1731,7 +1733,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A38" s="11" t="s">
         <v>102</v>
       </c>
@@ -1757,7 +1759,7 @@
         <v>0.36363636363636365</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A39" s="11" t="s">
         <v>11</v>
       </c>
@@ -1783,7 +1785,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A40" s="11" t="s">
         <v>12</v>
       </c>
@@ -1809,7 +1811,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>27</v>
       </c>
@@ -1818,22 +1820,22 @@
       </c>
       <c r="E41" s="12">
         <f t="shared" si="11"/>
-        <v>300</v>
+        <v>187.5</v>
       </c>
       <c r="F41" s="4">
         <f>1/$E41*1000</f>
-        <v>3.3333333333333335</v>
+        <v>5.333333333333333</v>
       </c>
       <c r="G41" s="9">
         <f>$E41*$B$3</f>
-        <v>6000</v>
+        <v>3750</v>
       </c>
       <c r="H41" s="9">
         <f t="shared" si="12"/>
-        <v>0.16666666666666669</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+        <v>0.26666666666666666</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A43" s="1" t="s">
         <v>18</v>
       </c>
@@ -1859,7 +1861,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>19</v>
       </c>
@@ -1890,7 +1892,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>106</v>
       </c>
@@ -1921,7 +1923,7 @@
         <v>5.4216867469879512E-2</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>105</v>
       </c>
@@ -1952,7 +1954,7 @@
         <v>4.6875000000000014E-2</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A48" s="1" t="s">
         <v>9</v>
       </c>
@@ -1978,7 +1980,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>112</v>
       </c>
@@ -2008,7 +2010,7 @@
         <v>0.10843373493975902</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>108</v>
       </c>
@@ -2038,7 +2040,7 @@
         <v>0.10843373493975902</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>111</v>
       </c>
@@ -2071,7 +2073,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A52" s="11" t="s">
         <v>32</v>
       </c>
@@ -2104,7 +2106,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A53" s="11" t="s">
         <v>33</v>
       </c>
@@ -2119,25 +2121,25 @@
       </c>
       <c r="E53" s="9">
         <f t="shared" si="13"/>
-        <v>4800</v>
+        <v>3000</v>
       </c>
       <c r="F53" s="9">
         <f t="shared" si="14"/>
-        <v>3.3333333333333335</v>
+        <v>5.333333333333333</v>
       </c>
       <c r="G53" s="12">
         <f t="shared" si="15"/>
-        <v>96000</v>
+        <v>60000</v>
       </c>
       <c r="H53" s="12">
         <f t="shared" si="16"/>
-        <v>0.16666666666666669</v>
+        <v>0.26666666666666666</v>
       </c>
       <c r="J53" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>31</v>
       </c>
@@ -2152,25 +2154,25 @@
       </c>
       <c r="E54" s="9">
         <f t="shared" si="13"/>
-        <v>2400</v>
+        <v>1500</v>
       </c>
       <c r="F54" s="9">
         <f t="shared" si="14"/>
-        <v>3.3333333333333335</v>
+        <v>5.333333333333333</v>
       </c>
       <c r="G54" s="9">
         <f t="shared" si="15"/>
-        <v>48000</v>
+        <v>30000</v>
       </c>
       <c r="H54" s="9">
         <f t="shared" si="16"/>
-        <v>0.16666666666666669</v>
+        <v>0.26666666666666666</v>
       </c>
       <c r="J54" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>13</v>
       </c>
@@ -2185,22 +2187,22 @@
       </c>
       <c r="E55" s="9">
         <f t="shared" si="13"/>
-        <v>19200</v>
+        <v>12000</v>
       </c>
       <c r="F55" s="9">
         <f t="shared" si="14"/>
-        <v>3.3333333333333335</v>
+        <v>5.333333333333333</v>
       </c>
       <c r="G55" s="9">
         <f t="shared" si="15"/>
-        <v>384000</v>
+        <v>240000</v>
       </c>
       <c r="H55" s="9">
         <f t="shared" si="16"/>
-        <v>0.16666666666666669</v>
-      </c>
-    </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+        <v>0.26666666666666666</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>21</v>
       </c>
@@ -2230,13 +2232,13 @@
         <v>0.18750000000000006</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.35">
       <c r="E57" s="9"/>
       <c r="F57" s="9"/>
       <c r="G57" s="9"/>
       <c r="H57" s="9"/>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A58" s="1" t="s">
         <v>49</v>
       </c>
@@ -2248,7 +2250,7 @@
       <c r="G58" s="9"/>
       <c r="H58" s="9"/>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>42</v>
       </c>
@@ -2263,7 +2265,7 @@
       <c r="G59" s="9"/>
       <c r="H59" s="9"/>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>43</v>
       </c>
@@ -2278,7 +2280,7 @@
       <c r="G60" s="9"/>
       <c r="H60" s="9"/>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>44</v>
       </c>
@@ -2293,7 +2295,7 @@
       <c r="G61" s="9"/>
       <c r="H61" s="9"/>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>50</v>
       </c>
@@ -2308,7 +2310,7 @@
       <c r="G62" s="9"/>
       <c r="H62" s="9"/>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>51</v>
       </c>
@@ -2323,7 +2325,7 @@
       <c r="G63" s="9"/>
       <c r="H63" s="9"/>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>52</v>
       </c>
@@ -2338,7 +2340,7 @@
       <c r="G64" s="9"/>
       <c r="H64" s="9"/>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>53</v>
       </c>
@@ -2353,7 +2355,7 @@
       <c r="G65" s="9"/>
       <c r="H65" s="9"/>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>54</v>
       </c>
@@ -2369,7 +2371,7 @@
       <c r="G66" s="9"/>
       <c r="H66" s="9"/>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>55</v>
       </c>
@@ -2385,7 +2387,7 @@
       <c r="G67" s="9"/>
       <c r="H67" s="9"/>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A69" s="1" t="s">
         <v>34</v>
       </c>
@@ -2414,7 +2416,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>67</v>
       </c>
@@ -2426,33 +2428,33 @@
       </c>
       <c r="D70">
         <f>($B$62+$B$61)*ROUND($B$3/VLOOKUP($B70,$A$20:$F$35,6,FALSE),0)-$C70</f>
-        <v>164</v>
+        <v>92</v>
       </c>
       <c r="E70" s="12">
         <f>$C70*VLOOKUP($B70,$A$20:$F$35,6,FALSE)</f>
-        <v>173.33333333333334</v>
+        <v>277.33333333333331</v>
       </c>
       <c r="F70" s="12">
         <f>$D70*VLOOKUP($B70,$A$20:$F$35,6,FALSE)</f>
-        <v>546.66666666666674</v>
+        <v>490.66666666666663</v>
       </c>
       <c r="G70" s="4">
         <f>$E70/$B$3</f>
-        <v>8.6666666666666679</v>
+        <v>13.866666666666665</v>
       </c>
       <c r="H70" s="4">
         <f>$F70/$B$3</f>
-        <v>27.333333333333336</v>
+        <v>24.533333333333331</v>
       </c>
       <c r="I70" s="4">
         <f>$G70+$H70</f>
-        <v>36</v>
+        <v>38.4</v>
       </c>
       <c r="K70" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>68</v>
       </c>
@@ -2464,33 +2466,33 @@
       </c>
       <c r="D71">
         <f>($B$63+$B$61)*ROUND($B$3/VLOOKUP($B71,$A$20:$F$35,6,FALSE),0)-$C71</f>
-        <v>147</v>
+        <v>75</v>
       </c>
       <c r="E71" s="12">
         <f t="shared" ref="E71:E77" si="17">$C71*VLOOKUP($B71,$A$20:$F$35,6,FALSE)</f>
-        <v>230</v>
+        <v>368</v>
       </c>
       <c r="F71" s="12">
         <f t="shared" ref="F71:F77" si="18">$D71*VLOOKUP($B71,$A$20:$F$35,6,FALSE)</f>
-        <v>490</v>
+        <v>400</v>
       </c>
       <c r="G71" s="4">
         <f t="shared" ref="G71:G77" si="19">$E71/$B$3</f>
-        <v>11.5</v>
+        <v>18.399999999999999</v>
       </c>
       <c r="H71" s="4">
         <f t="shared" ref="H71:H77" si="20">$F71/$B$3</f>
-        <v>24.5</v>
+        <v>20</v>
       </c>
       <c r="I71" s="4">
         <f t="shared" ref="I71:I77" si="21">$G71+$H71</f>
-        <v>36</v>
+        <v>38.4</v>
       </c>
       <c r="K71" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>69</v>
       </c>
@@ -2502,33 +2504,33 @@
       </c>
       <c r="D72">
         <f>($B$64+$B$66+$B$61)*ROUND($B$3/VLOOKUP($B72,$A$20:$F$35,6,FALSE),0)-$C72</f>
-        <v>584</v>
+        <v>372</v>
       </c>
       <c r="E72" s="12">
         <f t="shared" si="17"/>
-        <v>173.33333333333334</v>
+        <v>277.33333333333331</v>
       </c>
       <c r="F72" s="12">
         <f t="shared" si="18"/>
-        <v>1946.6666666666667</v>
+        <v>1984</v>
       </c>
       <c r="G72" s="4">
         <f t="shared" si="19"/>
-        <v>8.6666666666666679</v>
+        <v>13.866666666666665</v>
       </c>
       <c r="H72" s="4">
         <f t="shared" si="20"/>
-        <v>97.333333333333343</v>
+        <v>99.2</v>
       </c>
       <c r="I72" s="4">
         <f t="shared" si="21"/>
-        <v>106.00000000000001</v>
+        <v>113.06666666666666</v>
       </c>
       <c r="K72" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>70</v>
       </c>
@@ -2540,33 +2542,33 @@
       </c>
       <c r="D73">
         <f>($B$65+$B$67+$B$61)*ROUND($B$3/VLOOKUP($B73,$A$20:$F$35,6,FALSE),0)-$C73</f>
-        <v>441</v>
+        <v>271</v>
       </c>
       <c r="E73" s="12">
         <f t="shared" si="17"/>
-        <v>230</v>
+        <v>368</v>
       </c>
       <c r="F73" s="12">
         <f t="shared" si="18"/>
-        <v>1470</v>
+        <v>1445.3333333333333</v>
       </c>
       <c r="G73" s="4">
         <f t="shared" si="19"/>
-        <v>11.5</v>
+        <v>18.399999999999999</v>
       </c>
       <c r="H73" s="4">
         <f t="shared" si="20"/>
-        <v>73.5</v>
+        <v>72.266666666666666</v>
       </c>
       <c r="I73" s="4">
         <f t="shared" si="21"/>
-        <v>85</v>
+        <v>90.666666666666657</v>
       </c>
       <c r="K73" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>71</v>
       </c>
@@ -2578,33 +2580,33 @@
       </c>
       <c r="D74">
         <f>($B$62)*ROUND($B$3/VLOOKUP($B74,$A$20:$F$35,6,FALSE),0)-$C74</f>
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="E74" s="12">
         <f t="shared" si="17"/>
-        <v>160</v>
+        <v>256</v>
       </c>
       <c r="F74" s="12">
         <f t="shared" si="18"/>
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="G74" s="4">
         <f t="shared" si="19"/>
-        <v>8</v>
+        <v>12.8</v>
       </c>
       <c r="H74" s="4">
         <f t="shared" si="20"/>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="I74" s="4">
         <f t="shared" si="21"/>
-        <v>12</v>
+        <v>12.8</v>
       </c>
       <c r="K74" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>72</v>
       </c>
@@ -2616,33 +2618,33 @@
       </c>
       <c r="D75">
         <f>($B$63)*ROUND($B$3/VLOOKUP($B75,$A$20:$F$35,6,FALSE),0)-$C75</f>
-        <v>6</v>
+        <v>-18</v>
       </c>
       <c r="E75" s="12">
         <f t="shared" si="17"/>
-        <v>220</v>
+        <v>352</v>
       </c>
       <c r="F75" s="12">
         <f t="shared" si="18"/>
-        <v>20</v>
+        <v>-96</v>
       </c>
       <c r="G75" s="4">
         <f t="shared" si="19"/>
-        <v>11</v>
+        <v>17.600000000000001</v>
       </c>
       <c r="H75" s="4">
         <f t="shared" si="20"/>
-        <v>1</v>
+        <v>-4.8</v>
       </c>
       <c r="I75" s="4">
         <f t="shared" si="21"/>
-        <v>12</v>
+        <v>12.8</v>
       </c>
       <c r="K75" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>73</v>
       </c>
@@ -2654,33 +2656,33 @@
       </c>
       <c r="D76">
         <f>($B$64+$B$66)*ROUND($B$3/VLOOKUP($B76,$A$20:$F$35,6,FALSE),0)-$C76</f>
-        <v>444</v>
+        <v>280</v>
       </c>
       <c r="E76" s="12">
         <f t="shared" si="17"/>
-        <v>160</v>
+        <v>256</v>
       </c>
       <c r="F76" s="12">
         <f t="shared" si="18"/>
-        <v>1480</v>
+        <v>1493.3333333333333</v>
       </c>
       <c r="G76" s="4">
         <f t="shared" si="19"/>
-        <v>8</v>
+        <v>12.8</v>
       </c>
       <c r="H76" s="4">
         <f t="shared" si="20"/>
-        <v>74</v>
+        <v>74.666666666666657</v>
       </c>
       <c r="I76" s="4">
         <f t="shared" si="21"/>
-        <v>82</v>
+        <v>87.466666666666654</v>
       </c>
       <c r="K76" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>74</v>
       </c>
@@ -2692,56 +2694,56 @@
       </c>
       <c r="D77">
         <f>($B$65+$B$67)*ROUND($B$3/VLOOKUP($B77,$A$20:$F$35,6,FALSE),0)-$C77</f>
-        <v>300</v>
+        <v>178</v>
       </c>
       <c r="E77" s="12">
         <f t="shared" si="17"/>
-        <v>220</v>
+        <v>352</v>
       </c>
       <c r="F77" s="12">
         <f t="shared" si="18"/>
-        <v>1000</v>
+        <v>949.33333333333326</v>
       </c>
       <c r="G77" s="4">
         <f t="shared" si="19"/>
-        <v>11</v>
+        <v>17.600000000000001</v>
       </c>
       <c r="H77" s="4">
         <f t="shared" si="20"/>
-        <v>50</v>
+        <v>47.466666666666661</v>
       </c>
       <c r="I77" s="4">
         <f t="shared" si="21"/>
-        <v>61</v>
+        <v>65.066666666666663</v>
       </c>
       <c r="K77" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="79" spans="1:11" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:11" s="15" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A79" s="15" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="84" spans="1:1" s="15" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="90" spans="1:1" s="15" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="104" s="15" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="108" s="15" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="84" spans="1:1" s="15" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="90" spans="1:1" s="15" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="104" s="15" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="108" s="15" customFormat="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <pageMargins left="0.25" right="0.25" top="0.25" bottom="0.5" header="0.3" footer="0.3"/>
   <pageSetup scale="98" fitToHeight="0" orientation="portrait" r:id="rId1"/>
@@ -2754,7 +2756,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2766,7 +2768,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Fix spreadsheets, clocks.c, and trace/tools/ scripts for 250Mhz operation.
</commit_message>
<xml_diff>
--- a/system/clocks_sidewinder.xlsx
+++ b/system/clocks_sidewinder.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22827"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\macaraeg1\Projects\comp\repositories\lime_axi_delayv\system\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C656D14-A699-4451-8BE0-2CC645A1D1E9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F523E70-988F-48D3-A482-A0D7461309EE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13620" yWindow="0" windowWidth="18780" windowHeight="20750" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13620" yWindow="350" windowWidth="13630" windowHeight="20630" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -859,7 +859,7 @@
   <dimension ref="A1:K108"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1470,26 +1470,26 @@
         <v>89</v>
       </c>
       <c r="C28" s="3">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D28" s="3">
         <v>1</v>
       </c>
       <c r="E28" s="7">
         <f>VLOOKUP($B28,$A$11:$F$16,5,FALSE)/$C28/$D28</f>
-        <v>187.5</v>
+        <v>250</v>
       </c>
       <c r="F28" s="4">
         <f t="shared" si="4"/>
-        <v>5.333333333333333</v>
+        <v>4</v>
       </c>
       <c r="G28" s="9">
         <f t="shared" si="8"/>
-        <v>3750</v>
+        <v>5000</v>
       </c>
       <c r="H28" s="9">
         <f t="shared" si="9"/>
-        <v>0.26666666666666666</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.35">
@@ -1530,26 +1530,26 @@
         <v>89</v>
       </c>
       <c r="C30" s="3">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D30" s="3">
         <v>1</v>
       </c>
       <c r="E30" s="7">
         <f t="shared" ref="E30:E32" si="10">VLOOKUP($B30,$A$11:$F$16,5,FALSE)/$C30/$D30</f>
-        <v>187.5</v>
+        <v>250</v>
       </c>
       <c r="F30" s="4">
         <f t="shared" si="4"/>
-        <v>5.333333333333333</v>
+        <v>4</v>
       </c>
       <c r="G30" s="9">
         <f t="shared" si="8"/>
-        <v>3750</v>
+        <v>5000</v>
       </c>
       <c r="H30" s="9">
         <f t="shared" si="9"/>
-        <v>0.26666666666666666</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.35">
@@ -1820,19 +1820,19 @@
       </c>
       <c r="E41" s="12">
         <f t="shared" si="11"/>
-        <v>187.5</v>
+        <v>250</v>
       </c>
       <c r="F41" s="4">
         <f>1/$E41*1000</f>
-        <v>5.333333333333333</v>
+        <v>4</v>
       </c>
       <c r="G41" s="9">
         <f>$E41*$B$3</f>
-        <v>3750</v>
+        <v>5000</v>
       </c>
       <c r="H41" s="9">
         <f t="shared" si="12"/>
-        <v>0.26666666666666666</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.35">
@@ -2121,19 +2121,19 @@
       </c>
       <c r="E53" s="9">
         <f t="shared" si="13"/>
-        <v>3000</v>
+        <v>4000</v>
       </c>
       <c r="F53" s="9">
         <f t="shared" si="14"/>
-        <v>5.333333333333333</v>
+        <v>4</v>
       </c>
       <c r="G53" s="12">
         <f t="shared" si="15"/>
-        <v>60000</v>
+        <v>80000</v>
       </c>
       <c r="H53" s="12">
         <f t="shared" si="16"/>
-        <v>0.26666666666666666</v>
+        <v>0.2</v>
       </c>
       <c r="J53" t="s">
         <v>35</v>
@@ -2154,19 +2154,19 @@
       </c>
       <c r="E54" s="9">
         <f t="shared" si="13"/>
-        <v>1500</v>
+        <v>2000</v>
       </c>
       <c r="F54" s="9">
         <f t="shared" si="14"/>
-        <v>5.333333333333333</v>
+        <v>4</v>
       </c>
       <c r="G54" s="9">
         <f t="shared" si="15"/>
-        <v>30000</v>
+        <v>40000</v>
       </c>
       <c r="H54" s="9">
         <f t="shared" si="16"/>
-        <v>0.26666666666666666</v>
+        <v>0.2</v>
       </c>
       <c r="J54" t="s">
         <v>36</v>
@@ -2187,19 +2187,19 @@
       </c>
       <c r="E55" s="9">
         <f t="shared" si="13"/>
-        <v>12000</v>
+        <v>16000</v>
       </c>
       <c r="F55" s="9">
         <f t="shared" si="14"/>
-        <v>5.333333333333333</v>
+        <v>4</v>
       </c>
       <c r="G55" s="9">
         <f t="shared" si="15"/>
-        <v>240000</v>
+        <v>320000</v>
       </c>
       <c r="H55" s="9">
         <f t="shared" si="16"/>
-        <v>0.26666666666666666</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.35">
@@ -2428,27 +2428,27 @@
       </c>
       <c r="D70">
         <f>($B$62+$B$61)*ROUND($B$3/VLOOKUP($B70,$A$20:$F$35,6,FALSE),0)-$C70</f>
-        <v>92</v>
+        <v>128</v>
       </c>
       <c r="E70" s="12">
         <f>$C70*VLOOKUP($B70,$A$20:$F$35,6,FALSE)</f>
-        <v>277.33333333333331</v>
+        <v>208</v>
       </c>
       <c r="F70" s="12">
         <f>$D70*VLOOKUP($B70,$A$20:$F$35,6,FALSE)</f>
-        <v>490.66666666666663</v>
+        <v>512</v>
       </c>
       <c r="G70" s="4">
         <f>$E70/$B$3</f>
-        <v>13.866666666666665</v>
+        <v>10.4</v>
       </c>
       <c r="H70" s="4">
         <f>$F70/$B$3</f>
-        <v>24.533333333333331</v>
+        <v>25.6</v>
       </c>
       <c r="I70" s="4">
         <f>$G70+$H70</f>
-        <v>38.4</v>
+        <v>36</v>
       </c>
       <c r="K70" t="s">
         <v>75</v>
@@ -2466,27 +2466,27 @@
       </c>
       <c r="D71">
         <f>($B$63+$B$61)*ROUND($B$3/VLOOKUP($B71,$A$20:$F$35,6,FALSE),0)-$C71</f>
-        <v>75</v>
+        <v>111</v>
       </c>
       <c r="E71" s="12">
         <f t="shared" ref="E71:E77" si="17">$C71*VLOOKUP($B71,$A$20:$F$35,6,FALSE)</f>
-        <v>368</v>
+        <v>276</v>
       </c>
       <c r="F71" s="12">
         <f t="shared" ref="F71:F77" si="18">$D71*VLOOKUP($B71,$A$20:$F$35,6,FALSE)</f>
-        <v>400</v>
+        <v>444</v>
       </c>
       <c r="G71" s="4">
         <f t="shared" ref="G71:G77" si="19">$E71/$B$3</f>
-        <v>18.399999999999999</v>
+        <v>13.8</v>
       </c>
       <c r="H71" s="4">
         <f t="shared" ref="H71:H77" si="20">$F71/$B$3</f>
-        <v>20</v>
+        <v>22.2</v>
       </c>
       <c r="I71" s="4">
         <f t="shared" ref="I71:I77" si="21">$G71+$H71</f>
-        <v>38.4</v>
+        <v>36</v>
       </c>
       <c r="K71" t="s">
         <v>76</v>
@@ -2504,27 +2504,27 @@
       </c>
       <c r="D72">
         <f>($B$64+$B$66+$B$61)*ROUND($B$3/VLOOKUP($B72,$A$20:$F$35,6,FALSE),0)-$C72</f>
-        <v>372</v>
+        <v>478</v>
       </c>
       <c r="E72" s="12">
         <f t="shared" si="17"/>
-        <v>277.33333333333331</v>
+        <v>208</v>
       </c>
       <c r="F72" s="12">
         <f t="shared" si="18"/>
-        <v>1984</v>
+        <v>1912</v>
       </c>
       <c r="G72" s="4">
         <f t="shared" si="19"/>
-        <v>13.866666666666665</v>
+        <v>10.4</v>
       </c>
       <c r="H72" s="4">
         <f t="shared" si="20"/>
-        <v>99.2</v>
+        <v>95.6</v>
       </c>
       <c r="I72" s="4">
         <f t="shared" si="21"/>
-        <v>113.06666666666666</v>
+        <v>106</v>
       </c>
       <c r="K72" t="s">
         <v>77</v>
@@ -2542,27 +2542,27 @@
       </c>
       <c r="D73">
         <f>($B$65+$B$67+$B$61)*ROUND($B$3/VLOOKUP($B73,$A$20:$F$35,6,FALSE),0)-$C73</f>
-        <v>271</v>
+        <v>356</v>
       </c>
       <c r="E73" s="12">
         <f t="shared" si="17"/>
-        <v>368</v>
+        <v>276</v>
       </c>
       <c r="F73" s="12">
         <f t="shared" si="18"/>
-        <v>1445.3333333333333</v>
+        <v>1424</v>
       </c>
       <c r="G73" s="4">
         <f t="shared" si="19"/>
-        <v>18.399999999999999</v>
+        <v>13.8</v>
       </c>
       <c r="H73" s="4">
         <f t="shared" si="20"/>
-        <v>72.266666666666666</v>
+        <v>71.2</v>
       </c>
       <c r="I73" s="4">
         <f t="shared" si="21"/>
-        <v>90.666666666666657</v>
+        <v>85</v>
       </c>
       <c r="K73" t="s">
         <v>78</v>
@@ -2580,27 +2580,27 @@
       </c>
       <c r="D74">
         <f>($B$62)*ROUND($B$3/VLOOKUP($B74,$A$20:$F$35,6,FALSE),0)-$C74</f>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="E74" s="12">
         <f t="shared" si="17"/>
-        <v>256</v>
+        <v>192</v>
       </c>
       <c r="F74" s="12">
         <f t="shared" si="18"/>
-        <v>0</v>
+        <v>48</v>
       </c>
       <c r="G74" s="4">
         <f t="shared" si="19"/>
-        <v>12.8</v>
+        <v>9.6</v>
       </c>
       <c r="H74" s="4">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>2.4</v>
       </c>
       <c r="I74" s="4">
         <f t="shared" si="21"/>
-        <v>12.8</v>
+        <v>12</v>
       </c>
       <c r="K74" t="s">
         <v>79</v>
@@ -2618,27 +2618,27 @@
       </c>
       <c r="D75">
         <f>($B$63)*ROUND($B$3/VLOOKUP($B75,$A$20:$F$35,6,FALSE),0)-$C75</f>
-        <v>-18</v>
+        <v>-6</v>
       </c>
       <c r="E75" s="12">
         <f t="shared" si="17"/>
-        <v>352</v>
+        <v>264</v>
       </c>
       <c r="F75" s="12">
         <f t="shared" si="18"/>
-        <v>-96</v>
+        <v>-24</v>
       </c>
       <c r="G75" s="4">
         <f t="shared" si="19"/>
-        <v>17.600000000000001</v>
+        <v>13.2</v>
       </c>
       <c r="H75" s="4">
         <f t="shared" si="20"/>
-        <v>-4.8</v>
+        <v>-1.2</v>
       </c>
       <c r="I75" s="4">
         <f t="shared" si="21"/>
-        <v>12.8</v>
+        <v>12</v>
       </c>
       <c r="K75" t="s">
         <v>80</v>
@@ -2656,27 +2656,27 @@
       </c>
       <c r="D76">
         <f>($B$64+$B$66)*ROUND($B$3/VLOOKUP($B76,$A$20:$F$35,6,FALSE),0)-$C76</f>
-        <v>280</v>
+        <v>362</v>
       </c>
       <c r="E76" s="12">
         <f t="shared" si="17"/>
-        <v>256</v>
+        <v>192</v>
       </c>
       <c r="F76" s="12">
         <f t="shared" si="18"/>
-        <v>1493.3333333333333</v>
+        <v>1448</v>
       </c>
       <c r="G76" s="4">
         <f t="shared" si="19"/>
-        <v>12.8</v>
+        <v>9.6</v>
       </c>
       <c r="H76" s="4">
         <f t="shared" si="20"/>
-        <v>74.666666666666657</v>
+        <v>72.400000000000006</v>
       </c>
       <c r="I76" s="4">
         <f t="shared" si="21"/>
-        <v>87.466666666666654</v>
+        <v>82</v>
       </c>
       <c r="K76" t="s">
         <v>81</v>
@@ -2694,27 +2694,27 @@
       </c>
       <c r="D77">
         <f>($B$65+$B$67)*ROUND($B$3/VLOOKUP($B77,$A$20:$F$35,6,FALSE),0)-$C77</f>
-        <v>178</v>
+        <v>239</v>
       </c>
       <c r="E77" s="12">
         <f t="shared" si="17"/>
-        <v>352</v>
+        <v>264</v>
       </c>
       <c r="F77" s="12">
         <f t="shared" si="18"/>
-        <v>949.33333333333326</v>
+        <v>956</v>
       </c>
       <c r="G77" s="4">
         <f t="shared" si="19"/>
-        <v>17.600000000000001</v>
+        <v>13.2</v>
       </c>
       <c r="H77" s="4">
         <f t="shared" si="20"/>
-        <v>47.466666666666661</v>
+        <v>47.8</v>
       </c>
       <c r="I77" s="4">
         <f t="shared" si="21"/>
-        <v>65.066666666666663</v>
+        <v>61</v>
       </c>
       <c r="K77" t="s">
         <v>82</v>

</xml_diff>